<commit_message>
/DeepDanbooru/ /img/ static/bgm /数据库/
</commit_message>
<xml_diff>
--- a/开发队列/RandomPhotoProject开发队列.xlsx
+++ b/开发队列/RandomPhotoProject开发队列.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21277" windowHeight="8236"/>
+    <workbookView windowWidth="17383" windowHeight="8236"/>
   </bookViews>
   <sheets>
     <sheet name="仪表盘" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>RandomPhoto 开发队列仪表盘</t>
   </si>
@@ -53,10 +53,10 @@
     <t>问题描述</t>
   </si>
   <si>
-    <t>清理包含静态资源管理部门和ajax_hlper的相关代码</t>
+    <t>前端新增调试模式</t>
   </si>
   <si>
-    <t>前端新增调试模式</t>
+    <t>优化审核系统的布局</t>
   </si>
   <si>
     <t>加入用户系统防止爬虫</t>
@@ -74,7 +74,16 @@
     <t>RandomPhoto 发展问题队列</t>
   </si>
   <si>
+    <t>对服务端整个项目的tag进行重新审核，确保所有图片的tag不会有任何的问题</t>
+  </si>
+  <si>
+    <t>训练自定义模型</t>
+  </si>
+  <si>
     <t>RandomPhoto 需要重写队列</t>
+  </si>
+  <si>
+    <t>审核系统_图片审核需要重写</t>
   </si>
 </sst>
 </file>
@@ -855,7 +864,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -920,6 +929,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -989,7 +1001,6 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="00FEB300"/>
       <color rgb="00FFAD4B"/>
       <color rgb="00FFBE4B"/>
       <color rgb="00599200"/>
@@ -999,6 +1010,7 @@
       <color rgb="0000FBFE"/>
       <color rgb="000095F4"/>
       <color rgb="00FE8400"/>
+      <color rgb="0000FEF5"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1264,7 +1276,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1288,7 +1300,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1885,7 +1897,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1900,7 +1912,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:srgbClr val="00FEF5"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -2754,7 +2766,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3360,261 +3372,8 @@
       <c:pieChart>
         <c:varyColors val="1"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
-          <c:spPr/>
-          <c:explosion val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="0095F4"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00FBFE"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00F49B"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00AC45"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="149200"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="599200"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFBE4B"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FEB300"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF541F"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:srgbClr val="FE4444"/>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:srgbClr val="832B2B"/>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="1"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>发展问题队列!$B$27:$B$36</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
           <c:spPr/>
           <c:explosion val="0"/>
           <c:dPt>
@@ -3840,15 +3599,15 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>发展问题队列!$C$27:$C$36</c:f>
+              <c:f>发展问题队列!$C$26:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3870,6 +3629,265 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr/>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0095F4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00FBFE"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00F49B"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00AC45"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="149200"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="599200"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFBE4B"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FEB300"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF541F"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:srgbClr val="FE4444"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:srgbClr val="832B2B"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="1"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>发展问题队列!$B$26:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3896,196 +3914,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:legendEntry>
-        <c:idx val="0"/>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="1"/>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="2"/>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="3"/>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="4"/>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="5"/>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="6"/>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="7"/>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="8"/>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="9"/>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
@@ -6770,8 +6598,8 @@
   <sheetPr/>
   <dimension ref="B1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -6887,7 +6715,7 @@
       <c r="N6" s="19"/>
       <c r="O6" s="19"/>
       <c r="P6" s="19"/>
-      <c r="Q6" s="31"/>
+      <c r="Q6" s="32"/>
     </row>
     <row r="7" ht="17.25" spans="2:17">
       <c r="B7" s="20" t="s">
@@ -6901,7 +6729,7 @@
       </c>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="29"/>
+      <c r="I7" s="30"/>
       <c r="J7" s="21" t="s">
         <v>3</v>
       </c>
@@ -6913,7 +6741,7 @@
       </c>
       <c r="O7" s="21"/>
       <c r="P7" s="21"/>
-      <c r="Q7" s="32"/>
+      <c r="Q7" s="33"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="17.25" spans="2:17">
       <c r="B8" s="22"/>
@@ -6923,7 +6751,7 @@
       <c r="F8" s="23"/>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
-      <c r="I8" s="30"/>
+      <c r="I8" s="31"/>
       <c r="J8" s="23"/>
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
@@ -6931,7 +6759,7 @@
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
       <c r="P8" s="23"/>
-      <c r="Q8" s="33"/>
+      <c r="Q8" s="34"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="17.25" spans="2:17">
       <c r="B9" s="22"/>
@@ -6941,7 +6769,7 @@
       <c r="F9" s="23"/>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
-      <c r="I9" s="30"/>
+      <c r="I9" s="31"/>
       <c r="J9" s="23"/>
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
@@ -6949,7 +6777,7 @@
       <c r="N9" s="23"/>
       <c r="O9" s="23"/>
       <c r="P9" s="23"/>
-      <c r="Q9" s="33"/>
+      <c r="Q9" s="34"/>
     </row>
     <row r="10" spans="2:17">
       <c r="B10" s="8"/>
@@ -6971,66 +6799,66 @@
     </row>
     <row r="11" spans="2:17">
       <c r="B11" s="24"/>
-      <c r="Q11" s="34"/>
+      <c r="Q11" s="35"/>
     </row>
     <row r="12" spans="2:17">
       <c r="B12" s="24"/>
-      <c r="Q12" s="34"/>
+      <c r="Q12" s="35"/>
     </row>
     <row r="13" spans="2:17">
       <c r="B13" s="24"/>
-      <c r="Q13" s="34"/>
+      <c r="Q13" s="35"/>
     </row>
     <row r="14" spans="2:17">
       <c r="B14" s="24"/>
-      <c r="Q14" s="34"/>
+      <c r="Q14" s="35"/>
     </row>
     <row r="15" spans="2:17">
       <c r="B15" s="24"/>
-      <c r="Q15" s="34"/>
+      <c r="Q15" s="35"/>
     </row>
     <row r="16" spans="2:17">
       <c r="B16" s="24"/>
-      <c r="Q16" s="34"/>
+      <c r="Q16" s="35"/>
     </row>
     <row r="17" spans="2:17">
       <c r="B17" s="24"/>
-      <c r="Q17" s="34"/>
+      <c r="Q17" s="35"/>
     </row>
     <row r="18" spans="2:17">
       <c r="B18" s="24"/>
-      <c r="Q18" s="34"/>
+      <c r="Q18" s="35"/>
     </row>
     <row r="19" spans="2:17">
       <c r="B19" s="24"/>
-      <c r="Q19" s="34"/>
+      <c r="Q19" s="35"/>
     </row>
     <row r="20" spans="2:17">
       <c r="B20" s="24"/>
-      <c r="Q20" s="34"/>
+      <c r="Q20" s="35"/>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="24"/>
-      <c r="Q21" s="34"/>
+      <c r="Q21" s="35"/>
       <c r="S21" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="2:17">
       <c r="B22" s="24"/>
-      <c r="Q22" s="34"/>
+      <c r="Q22" s="35"/>
     </row>
     <row r="23" spans="2:17">
       <c r="B23" s="24"/>
-      <c r="Q23" s="34"/>
+      <c r="Q23" s="35"/>
     </row>
     <row r="24" spans="2:17">
       <c r="B24" s="24"/>
-      <c r="Q24" s="34"/>
+      <c r="Q24" s="35"/>
     </row>
     <row r="25" spans="2:17">
       <c r="B25" s="24"/>
-      <c r="Q25" s="34"/>
+      <c r="Q25" s="35"/>
     </row>
     <row r="26" ht="15.15" spans="2:17">
       <c r="B26" s="25"/>
@@ -7048,7 +6876,7 @@
       <c r="N26" s="26"/>
       <c r="O26" s="26"/>
       <c r="P26" s="26"/>
-      <c r="Q26" s="35"/>
+      <c r="Q26" s="36"/>
     </row>
     <row r="28" ht="4" customHeight="1"/>
     <row r="29" ht="21" customHeight="1" spans="2:5">
@@ -7056,14 +6884,15 @@
         <v>6</v>
       </c>
       <c r="C29" s="28"/>
-      <c r="D29" s="27">
+      <c r="D29" s="29">
         <f>COUNT(质量更新队列!B8:B24)+COUNT(BUG修复队列!B8:B24)+COUNT(发展问题队列!B8:B24)+COUNT(需要重写队列!B8:B24)</f>
-        <v>4</v>
-      </c>
-      <c r="E29" s="28"/>
+        <v>7</v>
+      </c>
+      <c r="E29" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="D29:E29"/>
     <mergeCell ref="B7:E9"/>
     <mergeCell ref="J7:M9"/>
     <mergeCell ref="N7:Q9"/>
@@ -7081,8 +6910,8 @@
   <sheetPr/>
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -7240,8 +7069,8 @@
     </row>
     <row r="8" s="2" customFormat="1" ht="15.55" spans="1:18">
       <c r="A8" s="9"/>
-      <c r="B8" s="8">
-        <v>10</v>
+      <c r="B8" s="9">
+        <v>8</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="10" t="s">
@@ -7264,8 +7093,8 @@
     </row>
     <row r="9" s="2" customFormat="1" ht="15.55" spans="1:18">
       <c r="A9" s="9"/>
-      <c r="B9" s="9">
-        <v>8</v>
+      <c r="B9" s="8">
+        <v>2</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="10" t="s">
@@ -7310,10 +7139,10 @@
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
     </row>
-    <row r="11" s="2" customFormat="1" ht="15.55" spans="1:18">
+    <row r="11" s="2" customFormat="1" spans="1:18">
       <c r="A11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -7604,7 +7433,7 @@
       </c>
       <c r="C27" s="12">
         <f>COUNTIF(B8:B24,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:3">
@@ -7676,13 +7505,13 @@
       </c>
       <c r="C35" s="2">
         <f>COUNTIF(B8:B24,10)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B8:B24">
-    <extLst/>
-  </autoFilter>
+  <sortState ref="B8:D10">
+    <sortCondition ref="B8" descending="1"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:R6"/>
   </mergeCells>
@@ -7725,7 +7554,7 @@
   <sheetPr/>
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A7" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -8085,6 +7914,7 @@
     </row>
     <row r="18" s="2" customFormat="1" ht="15.55" spans="1:18">
       <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="9"/>
@@ -8316,19 +8146,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:R6"/>
   </mergeCells>
-  <conditionalFormatting sqref="B8:B17">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18:B24">
+  <conditionalFormatting sqref="B8:B24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -8340,7 +8158,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:B24">
+  <conditionalFormatting sqref="B8:B10 B12:B24">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -8352,20 +8170,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B10 B12:B17">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B17 B18:B22 B23:B24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B22 B23:B24">
       <formula1>"10,9,8,7,6,5,4,3,2,1"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8379,8 +8185,8 @@
   <sheetPr/>
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -8536,9 +8342,13 @@
     </row>
     <row r="8" s="2" customFormat="1" ht="15.55" spans="1:18">
       <c r="A8" s="9"/>
-      <c r="B8" s="8"/>
+      <c r="B8" s="9">
+        <v>2</v>
+      </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
+      <c r="D8" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -8556,9 +8366,13 @@
     </row>
     <row r="9" s="2" customFormat="1" ht="15.55" spans="1:18">
       <c r="A9" s="9"/>
-      <c r="B9" s="8"/>
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
@@ -8596,7 +8410,6 @@
     </row>
     <row r="11" s="2" customFormat="1" ht="15.55" spans="1:18">
       <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="9"/>
@@ -8616,7 +8429,7 @@
     </row>
     <row r="12" s="2" customFormat="1" ht="15.55" spans="1:18">
       <c r="A12" s="9"/>
-      <c r="B12" s="2"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="9"/>
@@ -8880,7 +8693,7 @@
       </c>
       <c r="C26" s="12">
         <f>COUNTIF(B8:B24,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" s="2" customFormat="1" spans="2:3">
@@ -8889,7 +8702,7 @@
       </c>
       <c r="C27" s="12">
         <f>COUNTIF(B8:B24,2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" s="2" customFormat="1" spans="2:3">
@@ -8965,10 +8778,13 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="B8:D9">
+    <sortCondition ref="B8" descending="1"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:R6"/>
   </mergeCells>
-  <conditionalFormatting sqref="B9:B18">
+  <conditionalFormatting sqref="B8:B24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -8980,29 +8796,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8 B19:B24">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9:B11 B13:B18">
+  <conditionalFormatting sqref="B8:B10 B12:B24">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -9015,7 +8809,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8 B9:B18 B19:B22 B23:B24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B22 B23:B24">
       <formula1>"10,9,8,7,6,5,4,3,2,1"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9029,8 +8823,8 @@
   <sheetPr/>
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -9040,7 +8834,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -9186,9 +8980,13 @@
     </row>
     <row r="8" ht="15.55" spans="1:18">
       <c r="A8" s="9"/>
-      <c r="B8" s="8"/>
+      <c r="B8" s="8">
+        <v>4</v>
+      </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
+      <c r="D8" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -9206,7 +9004,7 @@
     </row>
     <row r="9" ht="15.55" spans="1:18">
       <c r="A9" s="9"/>
-      <c r="B9" s="8"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="9"/>
@@ -9246,7 +9044,6 @@
     </row>
     <row r="11" ht="15.55" spans="1:18">
       <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="9"/>
@@ -9266,6 +9063,7 @@
     </row>
     <row r="12" ht="15.55" spans="1:18">
       <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="9"/>
@@ -9556,7 +9354,7 @@
       </c>
       <c r="C29" s="2">
         <f>COUNTIF(B8:B24,4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:3">
@@ -9617,7 +9415,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:R6"/>
   </mergeCells>
-  <conditionalFormatting sqref="B9:B18">
+  <conditionalFormatting sqref="B8:B24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -9629,29 +9427,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8 B19:B24">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9:B11 B13:B18">
+  <conditionalFormatting sqref="B8:B10 B12:B24">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -9664,7 +9440,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8 B9:B18 B19:B22 B23:B24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B22 B23:B24">
       <formula1>"10,9,8,7,6,5,4,3,2,1"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>